<commit_message>
Still facing challenges with scanning
</commit_message>
<xml_diff>
--- a/reakai.xlsx
+++ b/reakai.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -206,9 +206,6 @@
   </si>
   <si>
     <t xml:space="preserve">freshpikt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6  00 1011 3 12988</t>
   </si>
   <si>
     <t xml:space="preserve">Baby Johnson</t>
@@ -637,7 +634,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1443,11 +1440,11 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="0" t="n">
+        <v>6001011312988</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>63</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>65</v>
@@ -1459,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>